<commit_message>
[FEATURE]: Se agrega módulo de login y sesion de usuarios.
</commit_message>
<xml_diff>
--- a/ChequesRecibidos.xlsx
+++ b/ChequesRecibidos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0323D8F4-8BFD-4B6F-AE77-9B5C05892AD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8329AE7D-D21C-4A64-9338-8E367A2C8D48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21168" yWindow="-100" windowWidth="21467" windowHeight="11443" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -442,7 +442,7 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -538,7 +538,7 @@
         <v>22</v>
       </c>
       <c r="M2">
-        <v>685544</v>
+        <v>111333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FEATURE]: Se implementa lógica para ENTRECUENTAS. Se corrigen incidencias en DIFERENCIAS.
</commit_message>
<xml_diff>
--- a/ChequesRecibidos.xlsx
+++ b/ChequesRecibidos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{806ED274-7A7E-42D9-9B25-A04FD2381181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{749D62A9-D9CD-4A44-A91F-6EDCB143F977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21168" yWindow="-100" windowWidth="21467" windowHeight="11443" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>ID</t>
   </si>
@@ -65,18 +65,39 @@
     <t>N° Documento</t>
   </si>
   <si>
+    <t>9500298</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>29743125</t>
+  </si>
+  <si>
+    <t>96509669</t>
+  </si>
+  <si>
+    <t>553710858954</t>
+  </si>
+  <si>
+    <t>182192</t>
+  </si>
+  <si>
+    <t>2024-10-07</t>
+  </si>
+  <si>
+    <t>CASTIGO</t>
+  </si>
+  <si>
+    <t>1 CUOTA</t>
+  </si>
+  <si>
     <t>17608148</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>29743125</t>
-  </si>
-  <si>
-    <t>96509669</t>
-  </si>
-  <si>
     <t>555581114451</t>
   </si>
   <si>
@@ -84,12 +105,6 @@
   </si>
   <si>
     <t>2024-10-10</t>
-  </si>
-  <si>
-    <t>CASTIGO</t>
-  </si>
-  <si>
-    <t>1 CUOTA</t>
   </si>
 </sst>
 </file>
@@ -436,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -533,6 +548,41 @@
       </c>
       <c r="M2">
         <v>456789</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>731942</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" t="s">
+        <v>21</v>
+      </c>
+      <c r="M3">
+        <v>123456</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FIX]: Se corrige logica para listar pareo cartola.
</commit_message>
<xml_diff>
--- a/ChequesRecibidos.xlsx
+++ b/ChequesRecibidos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{749D62A9-D9CD-4A44-A91F-6EDCB143F977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D635F784-80CD-4681-BAC4-8040AA5BBADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21168" yWindow="-100" windowWidth="21467" windowHeight="11443" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-100" yWindow="-100" windowWidth="21467" windowHeight="11443" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cheques" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="74">
   <si>
     <t>ID</t>
   </si>
@@ -65,46 +65,187 @@
     <t>N° Documento</t>
   </si>
   <si>
-    <t>9500298</t>
-  </si>
-  <si>
-    <t>6</t>
+    <t>11317290</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>CLAVERO VASQUEZ CECILIA DE LA CRUZ</t>
+  </si>
+  <si>
+    <t>61682420</t>
+  </si>
+  <si>
+    <t>96509669</t>
+  </si>
+  <si>
+    <t>555040421267</t>
+  </si>
+  <si>
+    <t>28963</t>
+  </si>
+  <si>
+    <t>2024-10-10</t>
+  </si>
+  <si>
+    <t>CASTIGO</t>
+  </si>
+  <si>
+    <t>1 CUOTA</t>
+  </si>
+  <si>
+    <t>18440875</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>BENITO AMOR MONCADA VALDIVIA</t>
   </si>
   <si>
     <t>29743125</t>
   </si>
   <si>
-    <t>96509669</t>
-  </si>
-  <si>
-    <t>553710858954</t>
-  </si>
-  <si>
-    <t>182192</t>
-  </si>
-  <si>
-    <t>2024-10-07</t>
-  </si>
-  <si>
-    <t>CASTIGO</t>
-  </si>
-  <si>
-    <t>1 CUOTA</t>
-  </si>
-  <si>
-    <t>17608148</t>
+    <t>96509660</t>
+  </si>
+  <si>
+    <t>209990602985</t>
+  </si>
+  <si>
+    <t>890291</t>
+  </si>
+  <si>
+    <t>2024-08-12</t>
+  </si>
+  <si>
+    <t>CONSUMO</t>
+  </si>
+  <si>
+    <t>VIGENTE</t>
+  </si>
+  <si>
+    <t>Rut Ordenante</t>
+  </si>
+  <si>
+    <t>DV</t>
+  </si>
+  <si>
+    <t>Banco Ordenante</t>
+  </si>
+  <si>
+    <t>Cuenta Ordenante</t>
+  </si>
+  <si>
+    <t>Monto</t>
+  </si>
+  <si>
+    <t>Operacion</t>
+  </si>
+  <si>
+    <t>Valor Cuota</t>
+  </si>
+  <si>
+    <t>Nombre Producto</t>
+  </si>
+  <si>
+    <t>N° Cuotas a pagar</t>
+  </si>
+  <si>
+    <t>Cuenta Beneficiario</t>
+  </si>
+  <si>
+    <t>13082181</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Banco Santander-Chile</t>
+  </si>
+  <si>
+    <t>77628746</t>
+  </si>
+  <si>
+    <t>235140240053</t>
+  </si>
+  <si>
+    <t>RENEGOCIACION</t>
+  </si>
+  <si>
+    <t>10320277</t>
+  </si>
+  <si>
+    <t>80675712</t>
+  </si>
+  <si>
+    <t>209991098982</t>
+  </si>
+  <si>
+    <t>17577704</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>Banco Falabella</t>
+  </si>
+  <si>
+    <t>17610001221</t>
+  </si>
+  <si>
+    <t>227610000225</t>
+  </si>
+  <si>
+    <t>REFINANCIAMIENTO</t>
+  </si>
+  <si>
+    <t>13268785</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>19990827010</t>
+  </si>
+  <si>
+    <t>209990432284</t>
+  </si>
+  <si>
+    <t>13685884</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>14800044702</t>
+  </si>
+  <si>
+    <t>204803109106</t>
+  </si>
+  <si>
+    <t>Nombre Deudor</t>
+  </si>
+  <si>
+    <t>13755821</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>555581114451</t>
-  </si>
-  <si>
-    <t>200669</t>
-  </si>
-  <si>
-    <t>2024-10-10</t>
+    <t>Banco Del Estado de Chile</t>
+  </si>
+  <si>
+    <t>36170508666</t>
+  </si>
+  <si>
+    <t>555581114360</t>
+  </si>
+  <si>
+    <t>CASTIGO BANCO</t>
+  </si>
+  <si>
+    <t>CATRILAF BARRAZA FABIOLA ANDREA</t>
   </si>
 </sst>
 </file>
@@ -454,7 +595,7 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -462,7 +603,7 @@
     <col min="1" max="1" width="8" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
     <col min="3" max="3" width="5" customWidth="1"/>
-    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="4" max="4" width="36" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
@@ -517,7 +658,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>731941</v>
+        <v>731947</v>
       </c>
       <c r="B2" t="s">
         <v>13</v>
@@ -525,64 +666,73 @@
       <c r="C2" t="s">
         <v>14</v>
       </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M2">
-        <v>456789</v>
+        <v>258852</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>731942</v>
+        <v>731949</v>
       </c>
       <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3" t="s">
+        <v>32</v>
+      </c>
+      <c r="L3" t="s">
         <v>22</v>
       </c>
-      <c r="C3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" t="s">
-        <v>26</v>
-      </c>
-      <c r="K3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L3" t="s">
-        <v>21</v>
-      </c>
       <c r="M3">
-        <v>123456</v>
+        <v>777777</v>
       </c>
     </row>
   </sheetData>
@@ -627,7 +777,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -635,25 +785,287 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="15" width="2" customWidth="1"/>
+    <col min="1" max="1" width="8" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="4" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="6" max="6" width="8" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
+    <col min="8" max="8" width="5" customWidth="1"/>
+    <col min="9" max="9" width="14" customWidth="1"/>
+    <col min="10" max="10" width="13" customWidth="1"/>
+    <col min="11" max="11" width="18" customWidth="1"/>
+    <col min="12" max="12" width="9" customWidth="1"/>
+    <col min="13" max="13" width="20" customWidth="1"/>
+    <col min="14" max="14" width="21" customWidth="1"/>
+    <col min="15" max="15" width="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="O1" s="1"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>731941</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2">
+        <v>137643</v>
+      </c>
+      <c r="G2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J2">
+        <v>137643</v>
+      </c>
+      <c r="K2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L2" t="s">
+        <v>32</v>
+      </c>
+      <c r="M2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>731942</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3">
+        <v>199707</v>
+      </c>
+      <c r="G3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J3">
+        <v>199707</v>
+      </c>
+      <c r="K3" t="s">
+        <v>31</v>
+      </c>
+      <c r="L3" t="s">
+        <v>32</v>
+      </c>
+      <c r="M3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>731943</v>
+      </c>
+      <c r="B4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4">
+        <v>229576</v>
+      </c>
+      <c r="G4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H4" t="s">
+        <v>53</v>
+      </c>
+      <c r="I4" t="s">
+        <v>56</v>
+      </c>
+      <c r="J4">
+        <v>229576</v>
+      </c>
+      <c r="K4" t="s">
+        <v>57</v>
+      </c>
+      <c r="L4" t="s">
+        <v>32</v>
+      </c>
+      <c r="M4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>731944</v>
+      </c>
+      <c r="B5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F5">
+        <v>249634</v>
+      </c>
+      <c r="G5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H5" t="s">
+        <v>59</v>
+      </c>
+      <c r="I5" t="s">
+        <v>61</v>
+      </c>
+      <c r="J5">
+        <v>249634</v>
+      </c>
+      <c r="K5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L5" t="s">
+        <v>32</v>
+      </c>
+      <c r="M5" t="s">
+        <v>22</v>
+      </c>
+      <c r="N5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>731945</v>
+      </c>
+      <c r="B6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F6">
+        <v>304019</v>
+      </c>
+      <c r="G6" t="s">
+        <v>62</v>
+      </c>
+      <c r="H6" t="s">
+        <v>63</v>
+      </c>
+      <c r="I6" t="s">
+        <v>65</v>
+      </c>
+      <c r="J6">
+        <v>304019</v>
+      </c>
+      <c r="K6" t="s">
+        <v>31</v>
+      </c>
+      <c r="L6" t="s">
+        <v>32</v>
+      </c>
+      <c r="M6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N6" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
@@ -663,7 +1075,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -671,26 +1083,118 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16" width="2" customWidth="1"/>
+    <col min="1" max="1" width="8" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="4" customWidth="1"/>
+    <col min="4" max="4" width="27" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="6" max="6" width="7" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
+    <col min="8" max="8" width="5" customWidth="1"/>
+    <col min="9" max="9" width="14" customWidth="1"/>
+    <col min="10" max="10" width="13" customWidth="1"/>
+    <col min="11" max="11" width="12" customWidth="1"/>
+    <col min="12" max="12" width="15" customWidth="1"/>
+    <col min="13" max="13" width="20" customWidth="1"/>
+    <col min="14" max="14" width="33" customWidth="1"/>
+    <col min="15" max="15" width="21" customWidth="1"/>
+    <col min="16" max="16" width="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="P1" s="1"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>731946</v>
+      </c>
+      <c r="B2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2">
+        <v>87435</v>
+      </c>
+      <c r="G2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I2" t="s">
+        <v>71</v>
+      </c>
+      <c r="J2">
+        <v>87435</v>
+      </c>
+      <c r="K2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" t="s">
+        <v>72</v>
+      </c>
+      <c r="M2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N2" t="s">
+        <v>73</v>
+      </c>
+      <c r="O2" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>

</xml_diff>

<commit_message>
[FIX]: Se corrige modulo de carga de transferencias recibidas.
</commit_message>
<xml_diff>
--- a/ChequesRecibidos.xlsx
+++ b/ChequesRecibidos.xlsx
@@ -1,30 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D635F784-80CD-4681-BAC4-8040AA5BBADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-100" yWindow="-100" windowWidth="21467" windowHeight="11443" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Cheques" sheetId="1" r:id="rId1"/>
-    <sheet name="CMR" sheetId="2" r:id="rId2"/>
-    <sheet name="Vigente" sheetId="3" r:id="rId3"/>
-    <sheet name="Castigo" sheetId="4" r:id="rId4"/>
-    <sheet name="Hipot" sheetId="5" r:id="rId5"/>
+    <sheet name="Cheques" sheetId="1" r:id="rId4"/>
+    <sheet name="CMR" sheetId="2" r:id="rId5"/>
+    <sheet name="Vigente" sheetId="3" r:id="rId6"/>
+    <sheet name="Castigo" sheetId="4" r:id="rId7"/>
+    <sheet name="Hipot" sheetId="5" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <definedNames/>
+  <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="98">
   <si>
     <t>ID</t>
   </si>
@@ -125,6 +120,84 @@
     <t>VIGENTE</t>
   </si>
   <si>
+    <t>7556522</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>EDILIO DEL TRANSITO ALVAREZ TALAMILLA</t>
+  </si>
+  <si>
+    <t>210021989816</t>
+  </si>
+  <si>
+    <t>146687</t>
+  </si>
+  <si>
+    <t>2024-09-27</t>
+  </si>
+  <si>
+    <t>AUTOMOTRIZ</t>
+  </si>
+  <si>
+    <t>JUDICIAL</t>
+  </si>
+  <si>
+    <t>14191212</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>PATRICIO ALEJANDRO HURTADO ALVAREZ</t>
+  </si>
+  <si>
+    <t>230017928138</t>
+  </si>
+  <si>
+    <t>165624</t>
+  </si>
+  <si>
+    <t>2024-05-09</t>
+  </si>
+  <si>
+    <t>RENEGOCIACION</t>
+  </si>
+  <si>
+    <t>11671345</t>
+  </si>
+  <si>
+    <t>FIERRO REYES CARLOS YASHIN</t>
+  </si>
+  <si>
+    <t>206005354319</t>
+  </si>
+  <si>
+    <t>281884</t>
+  </si>
+  <si>
+    <t>2024-06-05</t>
+  </si>
+  <si>
+    <t>17199914</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>CASTRO ARRIAGADA EVELIN NATALI</t>
+  </si>
+  <si>
+    <t>558330389530</t>
+  </si>
+  <si>
+    <t>66879</t>
+  </si>
+  <si>
+    <t>2024-10-21</t>
+  </si>
+  <si>
     <t>Rut Ordenante</t>
   </si>
   <si>
@@ -170,9 +243,6 @@
     <t>235140240053</t>
   </si>
   <si>
-    <t>RENEGOCIACION</t>
-  </si>
-  <si>
     <t>10320277</t>
   </si>
   <si>
@@ -201,9 +271,6 @@
   </si>
   <si>
     <t>13268785</t>
-  </si>
-  <si>
-    <t>4</t>
   </si>
   <si>
     <t>19990827010</t>
@@ -251,15 +318,23 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -274,34 +349,24 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
 </styleSheet>
 </file>
 
@@ -591,31 +656,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
+  <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="8" customWidth="1"/>
-    <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="5" customWidth="1"/>
-    <col min="4" max="4" width="36" customWidth="1"/>
-    <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="14" customWidth="1"/>
-    <col min="8" max="8" width="10" customWidth="1"/>
-    <col min="9" max="9" width="12" customWidth="1"/>
-    <col min="10" max="10" width="13" customWidth="1"/>
-    <col min="11" max="11" width="9" customWidth="1"/>
-    <col min="12" max="12" width="12" customWidth="1"/>
-    <col min="13" max="13" width="15" customWidth="1"/>
+    <col min="1" max="1" width="8" customWidth="true" style="0"/>
+    <col min="2" max="2" width="13" customWidth="true" style="0"/>
+    <col min="3" max="3" width="5" customWidth="true" style="0"/>
+    <col min="4" max="4" width="39" customWidth="true" style="0"/>
+    <col min="5" max="5" width="12" customWidth="true" style="0"/>
+    <col min="6" max="6" width="13" customWidth="true" style="0"/>
+    <col min="7" max="7" width="14" customWidth="true" style="0"/>
+    <col min="8" max="8" width="10" customWidth="true" style="0"/>
+    <col min="9" max="9" width="12" customWidth="true" style="0"/>
+    <col min="10" max="10" width="15" customWidth="true" style="0"/>
+    <col min="11" max="11" width="10" customWidth="true" style="0"/>
+    <col min="12" max="12" width="12" customWidth="true" style="0"/>
+    <col min="13" max="13" width="15" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -656,7 +724,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13">
       <c r="A2">
         <v>731947</v>
       </c>
@@ -684,6 +752,7 @@
       <c r="I2" t="s">
         <v>20</v>
       </c>
+      <c r="J2"/>
       <c r="K2" t="s">
         <v>21</v>
       </c>
@@ -694,7 +763,7 @@
         <v>258852</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13">
       <c r="A3">
         <v>731949</v>
       </c>
@@ -735,26 +804,206 @@
         <v>777777</v>
       </c>
     </row>
+    <row r="4" spans="1:13">
+      <c r="A4">
+        <v>731950</v>
+      </c>
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I4" t="s">
+        <v>38</v>
+      </c>
+      <c r="J4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L4" t="s">
+        <v>22</v>
+      </c>
+      <c r="M4"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5">
+        <v>731951</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5" t="s">
+        <v>46</v>
+      </c>
+      <c r="J5" t="s">
+        <v>47</v>
+      </c>
+      <c r="K5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M5"/>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6">
+        <v>731952</v>
+      </c>
+      <c r="B6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6" t="s">
+        <v>51</v>
+      </c>
+      <c r="I6" t="s">
+        <v>52</v>
+      </c>
+      <c r="J6" t="s">
+        <v>31</v>
+      </c>
+      <c r="K6" t="s">
+        <v>32</v>
+      </c>
+      <c r="L6" t="s">
+        <v>22</v>
+      </c>
+      <c r="M6"/>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7">
+        <v>731953</v>
+      </c>
+      <c r="B7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" t="s">
+        <v>56</v>
+      </c>
+      <c r="H7" t="s">
+        <v>57</v>
+      </c>
+      <c r="I7" t="s">
+        <v>58</v>
+      </c>
+      <c r="J7"/>
+      <c r="K7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L7" t="s">
+        <v>22</v>
+      </c>
+      <c r="M7"/>
+    </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+  <tableParts count="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
   <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="13" width="2" customWidth="1"/>
+    <col min="1" max="1" width="2" customWidth="true" style="0"/>
+    <col min="2" max="2" width="2" customWidth="true" style="0"/>
+    <col min="3" max="3" width="2" customWidth="true" style="0"/>
+    <col min="4" max="4" width="2" customWidth="true" style="0"/>
+    <col min="5" max="5" width="2" customWidth="true" style="0"/>
+    <col min="6" max="6" width="2" customWidth="true" style="0"/>
+    <col min="7" max="7" width="2" customWidth="true" style="0"/>
+    <col min="8" max="8" width="2" customWidth="true" style="0"/>
+    <col min="9" max="9" width="2" customWidth="true" style="0"/>
+    <col min="10" max="10" width="2" customWidth="true" style="0"/>
+    <col min="11" max="11" width="2" customWidth="true" style="0"/>
+    <col min="12" max="12" width="2" customWidth="true" style="0"/>
+    <col min="13" max="13" width="2" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -770,56 +1019,70 @@
       <c r="M1" s="1"/>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+  <tableParts count="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
   <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="8" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="4" customWidth="1"/>
-    <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="8" customWidth="1"/>
-    <col min="7" max="7" width="13" customWidth="1"/>
-    <col min="8" max="8" width="5" customWidth="1"/>
-    <col min="9" max="9" width="14" customWidth="1"/>
-    <col min="10" max="10" width="13" customWidth="1"/>
-    <col min="11" max="11" width="18" customWidth="1"/>
-    <col min="12" max="12" width="9" customWidth="1"/>
-    <col min="13" max="13" width="20" customWidth="1"/>
-    <col min="14" max="14" width="21" customWidth="1"/>
-    <col min="15" max="15" width="2" customWidth="1"/>
+    <col min="1" max="1" width="8" customWidth="true" style="0"/>
+    <col min="2" max="2" width="15" customWidth="true" style="0"/>
+    <col min="3" max="3" width="4" customWidth="true" style="0"/>
+    <col min="4" max="4" width="23" customWidth="true" style="0"/>
+    <col min="5" max="5" width="18" customWidth="true" style="0"/>
+    <col min="6" max="6" width="8" customWidth="true" style="0"/>
+    <col min="7" max="7" width="13" customWidth="true" style="0"/>
+    <col min="8" max="8" width="5" customWidth="true" style="0"/>
+    <col min="9" max="9" width="14" customWidth="true" style="0"/>
+    <col min="10" max="10" width="13" customWidth="true" style="0"/>
+    <col min="11" max="11" width="18" customWidth="true" style="0"/>
+    <col min="12" max="12" width="9" customWidth="true" style="0"/>
+    <col min="13" max="13" width="20" customWidth="true" style="0"/>
+    <col min="14" max="14" width="21" customWidth="true" style="0"/>
+    <col min="15" max="15" width="2" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>1</v>
@@ -828,58 +1091,58 @@
         <v>2</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="O1" s="1"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15">
       <c r="A2">
         <v>731941</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="E2" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
       <c r="F2">
         <v>137643</v>
       </c>
       <c r="G2" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="H2" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="I2" t="s">
-        <v>47</v>
+        <v>73</v>
       </c>
       <c r="J2">
         <v>137643</v>
       </c>
       <c r="K2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L2" t="s">
         <v>32</v>
@@ -890,34 +1153,35 @@
       <c r="N2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O2"/>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3">
         <v>731942</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>74</v>
       </c>
       <c r="C3" t="s">
         <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="E3" t="s">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="F3">
         <v>199707</v>
       </c>
       <c r="G3" t="s">
-        <v>49</v>
+        <v>74</v>
       </c>
       <c r="H3" t="s">
         <v>24</v>
       </c>
       <c r="I3" t="s">
-        <v>51</v>
+        <v>76</v>
       </c>
       <c r="J3">
         <v>199707</v>
@@ -934,40 +1198,41 @@
       <c r="N3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O3"/>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4">
         <v>731943</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
+        <v>77</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>78</v>
       </c>
       <c r="D4" t="s">
-        <v>54</v>
+        <v>79</v>
       </c>
       <c r="E4" t="s">
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="F4">
         <v>229576</v>
       </c>
       <c r="G4" t="s">
-        <v>52</v>
+        <v>77</v>
       </c>
       <c r="H4" t="s">
-        <v>53</v>
+        <v>78</v>
       </c>
       <c r="I4" t="s">
-        <v>56</v>
+        <v>81</v>
       </c>
       <c r="J4">
         <v>229576</v>
       </c>
       <c r="K4" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="L4" t="s">
         <v>32</v>
@@ -978,34 +1243,35 @@
       <c r="N4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O4"/>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5">
         <v>731944</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="C5" t="s">
-        <v>59</v>
+        <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>54</v>
+        <v>79</v>
       </c>
       <c r="E5" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="F5">
         <v>249634</v>
       </c>
       <c r="G5" t="s">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="H5" t="s">
-        <v>59</v>
+        <v>34</v>
       </c>
       <c r="I5" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="J5">
         <v>249634</v>
@@ -1022,34 +1288,35 @@
       <c r="N5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O5"/>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6">
         <v>731945</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="C6" t="s">
-        <v>63</v>
+        <v>87</v>
       </c>
       <c r="D6" t="s">
-        <v>54</v>
+        <v>79</v>
       </c>
       <c r="E6" t="s">
-        <v>64</v>
+        <v>88</v>
       </c>
       <c r="F6">
         <v>304019</v>
       </c>
       <c r="G6" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="H6" t="s">
-        <v>63</v>
+        <v>87</v>
       </c>
       <c r="I6" t="s">
-        <v>65</v>
+        <v>89</v>
       </c>
       <c r="J6">
         <v>304019</v>
@@ -1066,59 +1333,74 @@
       <c r="N6" t="s">
         <v>26</v>
       </c>
+      <c r="O6"/>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+  <tableParts count="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="8" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="4" customWidth="1"/>
-    <col min="4" max="4" width="27" customWidth="1"/>
-    <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="7" customWidth="1"/>
-    <col min="7" max="7" width="13" customWidth="1"/>
-    <col min="8" max="8" width="5" customWidth="1"/>
-    <col min="9" max="9" width="14" customWidth="1"/>
-    <col min="10" max="10" width="13" customWidth="1"/>
-    <col min="11" max="11" width="12" customWidth="1"/>
-    <col min="12" max="12" width="15" customWidth="1"/>
-    <col min="13" max="13" width="20" customWidth="1"/>
-    <col min="14" max="14" width="33" customWidth="1"/>
-    <col min="15" max="15" width="21" customWidth="1"/>
-    <col min="16" max="16" width="2" customWidth="1"/>
+    <col min="1" max="1" width="8" customWidth="true" style="0"/>
+    <col min="2" max="2" width="15" customWidth="true" style="0"/>
+    <col min="3" max="3" width="4" customWidth="true" style="0"/>
+    <col min="4" max="4" width="27" customWidth="true" style="0"/>
+    <col min="5" max="5" width="18" customWidth="true" style="0"/>
+    <col min="6" max="6" width="7" customWidth="true" style="0"/>
+    <col min="7" max="7" width="13" customWidth="true" style="0"/>
+    <col min="8" max="8" width="5" customWidth="true" style="0"/>
+    <col min="9" max="9" width="14" customWidth="true" style="0"/>
+    <col min="10" max="10" width="13" customWidth="true" style="0"/>
+    <col min="11" max="11" width="12" customWidth="true" style="0"/>
+    <col min="12" max="12" width="15" customWidth="true" style="0"/>
+    <col min="13" max="13" width="20" customWidth="true" style="0"/>
+    <col min="14" max="14" width="33" customWidth="true" style="0"/>
+    <col min="15" max="15" width="21" customWidth="true" style="0"/>
+    <col min="16" max="16" width="2" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>1</v>
@@ -1127,10 +1409,10 @@
         <v>2</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>11</v>
@@ -1139,43 +1421,43 @@
         <v>10</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>66</v>
+        <v>90</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="P1" s="1"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16">
       <c r="A2">
         <v>731946</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
       <c r="C2" t="s">
-        <v>68</v>
+        <v>92</v>
       </c>
       <c r="D2" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="E2" t="s">
-        <v>70</v>
+        <v>94</v>
       </c>
       <c r="F2">
         <v>87435</v>
       </c>
       <c r="G2" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
       <c r="H2" t="s">
-        <v>68</v>
+        <v>92</v>
       </c>
       <c r="I2" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="J2">
         <v>87435</v>
@@ -1184,38 +1466,66 @@
         <v>22</v>
       </c>
       <c r="L2" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="M2" t="s">
         <v>22</v>
       </c>
       <c r="N2" t="s">
-        <v>73</v>
+        <v>97</v>
       </c>
       <c r="O2" t="s">
         <v>16</v>
       </c>
+      <c r="P2"/>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+  <tableParts count="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
   <dimension ref="A1:N1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="14" width="2" customWidth="1"/>
+    <col min="1" max="1" width="2" customWidth="true" style="0"/>
+    <col min="2" max="2" width="2" customWidth="true" style="0"/>
+    <col min="3" max="3" width="2" customWidth="true" style="0"/>
+    <col min="4" max="4" width="2" customWidth="true" style="0"/>
+    <col min="5" max="5" width="2" customWidth="true" style="0"/>
+    <col min="6" max="6" width="2" customWidth="true" style="0"/>
+    <col min="7" max="7" width="2" customWidth="true" style="0"/>
+    <col min="8" max="8" width="2" customWidth="true" style="0"/>
+    <col min="9" max="9" width="2" customWidth="true" style="0"/>
+    <col min="10" max="10" width="2" customWidth="true" style="0"/>
+    <col min="11" max="11" width="2" customWidth="true" style="0"/>
+    <col min="12" max="12" width="2" customWidth="true" style="0"/>
+    <col min="13" max="13" width="2" customWidth="true" style="0"/>
+    <col min="14" max="14" width="2" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1232,7 +1542,18 @@
       <c r="N1" s="1"/>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+  <tableParts count="0"/>
 </worksheet>
 </file>
</xml_diff>